<commit_message>
add virtual service to simulate something
</commit_message>
<xml_diff>
--- a/tools/xlsx2xml/xlsx/VirtualService/VirtualConfig.xlsx
+++ b/tools/xlsx2xml/xlsx/VirtualService/VirtualConfig.xlsx
@@ -7,7 +7,7 @@
     <workbookView windowWidth="26880" windowHeight="11040"/>
   </bookViews>
   <sheets>
-    <sheet name="LocalServerConfig" sheetId="1" r:id="rId1"/>
+    <sheet name="VirtualServiceConfig" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -66,8 +66,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -75,61 +112,86 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -140,68 +202,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -212,6 +212,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -224,13 +248,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,25 +350,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,127 +386,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -403,6 +403,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -417,17 +432,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -449,8 +453,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -475,7 +481,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -489,17 +495,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -511,10 +511,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -523,7 +523,7 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -532,124 +532,124 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="3" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>

</xml_diff>